<commit_message>
WIP: local changes before merge
</commit_message>
<xml_diff>
--- a/backend/immediate_feedback.xlsx
+++ b/backend/immediate_feedback.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -513,6 +513,64 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>689580fc-3200-4fe8-a3b6-02eb7cb60de4</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-03-23 00:41:49</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+You are a change management expert helping companies adopt new technologies using structured frameworks.
+A company wants to adopt a new technology: grok
+They want to follow the adkar framework.
+Give a clear, step-by-step guide tailored to ops. using the adkar model. Make it practical and actionable.
+Use numbered steps and keep the tone helpful.
+Also include a list of common technical FAQs regarding the technology and answers to help employees understand the change process.
+</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>make it easier for ops</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>4a1f6efc-bf0c-40b3-b27e-cfcb56cc26e5</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2025-03-23 00:43:42</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+You are a change management expert helping companies adopt new technologies using structured frameworks.
+A company wants to adopt a new technology: grok
+They want to follow the adkar framework.
+Give a clear, step-by-step guide tailored to ops. using the adkar model. Make it practical and actionable.
+Use numbered steps and keep the tone helpful.
+Also include a list of common technical FAQs regarding the technology and answers to help employees understand the change process.
+</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>use levin</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>